<commit_message>
Updated formspecs (added setting: framework_variant, solving appdesigner crash)
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E817130D-31DA-470E-BC1C-C21F98CE69ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A34F71-7245-4F2A-8657-349F555AA58F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="222">
   <si>
     <t>clause</t>
   </si>
@@ -639,9 +639,6 @@
     <t>user_branch</t>
   </si>
   <si>
-    <t>Choose a test form</t>
-  </si>
-  <si>
     <t>else</t>
   </si>
   <si>
@@ -712,6 +709,12 @@
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('MIFVAC')</t>
+  </si>
+  <si>
+    <t>Choose a form</t>
+  </si>
+  <si>
+    <t>framework_variant</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1062,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B793DC04-5EE8-4C44-A7FC-F90344029075}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,18 +1133,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>20190520</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>20190521</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1175,6 +1178,11 @@
       </c>
       <c r="F7" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1186,9 +1194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1214,58 +1220,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" t="s">
         <v>204</v>
       </c>
-      <c r="B2" t="s">
-        <v>205</v>
-      </c>
       <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" t="s">
         <v>213</v>
-      </c>
-      <c r="D2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" t="s">
         <v>207</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>208</v>
-      </c>
-      <c r="D3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" t="s">
         <v>215</v>
-      </c>
-      <c r="D5" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1277,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46EC045-695E-47E3-9856-F3F6A59BF71E}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,117 +1334,117 @@
         <v>195</v>
       </c>
       <c r="F3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G5" t="s">
         <v>198</v>
-      </c>
-      <c r="G5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" t="s">
         <v>202</v>
-      </c>
-      <c r="G9" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" t="s">
         <v>202</v>
-      </c>
-      <c r="G12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E15" t="s">
+        <v>201</v>
+      </c>
+      <c r="G15" t="s">
         <v>202</v>
-      </c>
-      <c r="G15" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G18" t="s">
         <v>202</v>
-      </c>
-      <c r="G18" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added custom prompt type: adate
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A34F71-7245-4F2A-8657-349F555AA58F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E338F6A-F7D0-4CB4-81DD-AEEA0338E3EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="227">
   <si>
     <t>clause</t>
   </si>
@@ -715,6 +715,21 @@
   </si>
   <si>
     <t>framework_variant</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('TEST')</t>
+  </si>
+  <si>
+    <t>Open test</t>
+  </si>
+  <si>
+    <t>TEST Form</t>
+  </si>
+  <si>
+    <t>Test formulario</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B793DC04-5EE8-4C44-A7FC-F90344029075}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,9 +1207,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1274,6 +1291,20 @@
         <v>215</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1281,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46EC045-695E-47E3-9856-F3F6A59BF71E}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,6 +1478,27 @@
         <v>200</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1456,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A43F1AA-AE9E-40A3-94B1-695B21603B14}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Default language: Portuguese + smaller changes
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A34F71-7245-4F2A-8657-349F555AA58F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EDE110-B57F-4E4B-B036-50C7CA498FC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="223">
   <si>
     <t>clause</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>text.default</t>
-  </si>
-  <si>
-    <t>text.portuguese</t>
   </si>
   <si>
     <t>constraint_message</t>
@@ -576,15 +573,9 @@
     <t>Options</t>
   </si>
   <si>
-    <t>display.title.text.portuguese</t>
-  </si>
-  <si>
     <t>display.locale.text</t>
   </si>
   <si>
-    <t>display.locale.text.portuguese</t>
-  </si>
-  <si>
     <t>Opções</t>
   </si>
   <si>
@@ -603,9 +594,6 @@
     <t>default</t>
   </si>
   <si>
-    <t>portuguese</t>
-  </si>
-  <si>
     <t>choice_list_name</t>
   </si>
   <si>
@@ -715,6 +703,21 @@
   </si>
   <si>
     <t>framework_variant</t>
+  </si>
+  <si>
+    <t>display.title.text.english</t>
+  </si>
+  <si>
+    <t>display.locale.text.english</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>text.english</t>
+  </si>
+  <si>
+    <t>Missing</t>
   </si>
 </sst>
 </file>
@@ -737,12 +740,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -766,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -779,6 +788,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B793DC04-5EE8-4C44-A7FC-F90344029075}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1111,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1111,16 +1123,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,37 +1164,37 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" t="s">
         <v>179</v>
-      </c>
-      <c r="F6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1194,7 +1206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1206,72 +1220,72 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" t="s">
         <v>203</v>
       </c>
-      <c r="B3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" t="s">
-        <v>207</v>
-      </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" t="s">
         <v>211</v>
-      </c>
-      <c r="C5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D5" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1300,151 +1314,151 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G18" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1456,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A43F1AA-AE9E-40A3-94B1-695B21603B14}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,621 +1486,648 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
+      <c r="C5" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
+      <c r="C6" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
+      <c r="C7" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
+      <c r="C13" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
+      <c r="C14" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>47</v>
+      <c r="C15" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
+      <c r="C16" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>51</v>
+      <c r="C17" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" t="s">
         <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" t="s">
         <v>77</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>101</v>
+      <c r="C34" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Link Between MIFCRIANCA And MIFCRIANCA_VISIT
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252A3D6D-2586-4412-AD6C-EAD314AB6635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C939245-646C-4048-A9FD-B336928EFC03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="246">
   <si>
     <t>clause</t>
   </si>
@@ -778,6 +778,15 @@
   </si>
   <si>
     <t>Child visit</t>
+  </si>
+  <si>
+    <t>MIFCRIANCA</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MIFCRIANCA')</t>
+  </si>
+  <si>
+    <t>CHILD</t>
   </si>
 </sst>
 </file>
@@ -1264,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,6 +1427,20 @@
         <v>242</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" t="s">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1425,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46EC045-695E-47E3-9856-F3F6A59BF71E}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1703,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>240</v>
       </c>
@@ -1691,8 +1714,29 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E36" t="s">
+        <v>197</v>
+      </c>
+      <c r="G36" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>196</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Framework And Added Bandim Logo
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C939245-646C-4048-A9FD-B336928EFC03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6110D18-A561-44B0-B36B-00FA82324FBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
   <si>
     <t>clause</t>
   </si>
@@ -669,24 +669,6 @@
     <t>'?' + odkSurvey.getHashString('MIFVISIT')</t>
   </si>
   <si>
-    <t>MIFSCAR</t>
-  </si>
-  <si>
-    <t>Woman in the fertile age - core</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - núcleo</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - cicatrizes</t>
-  </si>
-  <si>
-    <t>Woman in the fertile age - scars</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFSCAR')</t>
-  </si>
-  <si>
     <t>Choose a form</t>
   </si>
   <si>
@@ -717,76 +699,88 @@
     <t>Test Formulario</t>
   </si>
   <si>
-    <t>MIFVISIT_CORE</t>
-  </si>
-  <si>
-    <t>Woman in the fertile age - visit_core</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - visitas_núcleo</t>
-  </si>
-  <si>
-    <t>MIFSES</t>
-  </si>
-  <si>
-    <t>MIFGRAVIDA</t>
-  </si>
-  <si>
-    <t>MIFGRAVIDA_VISIT</t>
-  </si>
-  <si>
-    <t>Woman in the fertile age - pregnants</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - grávidas</t>
-  </si>
-  <si>
-    <t>Woman in the fertile age - pregnants_visits</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - grávidas_visitas</t>
-  </si>
-  <si>
-    <t>Woman in the fertile age - SES</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - SES</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFVISIT_CORE')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFSES')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFGRAVIDA')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFGRAVIDA_VISIT')</t>
-  </si>
-  <si>
     <t>'?' + odkSurvey.getHashString('TEST')</t>
   </si>
   <si>
-    <t>MIFCRIANCA_VISIT</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFCRIANCA_VISIT')</t>
-  </si>
-  <si>
     <t>Child Visit</t>
   </si>
   <si>
     <t>Child visit</t>
   </si>
   <si>
-    <t>MIFCRIANCA</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIFCRIANCA')</t>
-  </si>
-  <si>
     <t>CHILD</t>
+  </si>
+  <si>
+    <t>SCAR</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('SCAR')</t>
+  </si>
+  <si>
+    <t>CRIANCA</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('CRIANCA')</t>
+  </si>
+  <si>
+    <t>GRAVIDA</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('GRAVIDA')</t>
+  </si>
+  <si>
+    <t>GRAVIDA_VISIT</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('GRAVIDA_VISIT')</t>
+  </si>
+  <si>
+    <t>CRIANCA_VISIT</t>
+  </si>
+  <si>
+    <t>SES</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('SES')</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('CRIANCA_VISIT')</t>
+  </si>
+  <si>
+    <t>VAC</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('VAC')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woman in the fertile age </t>
+  </si>
+  <si>
+    <t>Vaccine</t>
+  </si>
+  <si>
+    <t>Scars</t>
+  </si>
+  <si>
+    <t>Cicatrizes</t>
+  </si>
+  <si>
+    <t>Mulher na idade fertil - visitas</t>
+  </si>
+  <si>
+    <t>Mulher na idade fertil</t>
+  </si>
+  <si>
+    <t>Pregnant</t>
+  </si>
+  <si>
+    <t>Grávidas</t>
+  </si>
+  <si>
+    <t>Pregnants_visits</t>
+  </si>
+  <si>
+    <t>Grávidas_visitas</t>
   </si>
 </sst>
 </file>
@@ -1192,13 +1186,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>174</v>
@@ -1252,7 +1246,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E7" t="s">
         <v>176</v>
@@ -1263,7 +1257,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1270,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1289,7 @@
         <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1309,10 +1303,10 @@
         <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1334,13 +1328,13 @@
         <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1348,13 +1342,13 @@
         <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1362,13 +1356,13 @@
         <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1376,13 +1370,13 @@
         <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="D7" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1390,13 +1384,13 @@
         <v>199</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1404,13 +1398,13 @@
         <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1418,13 +1412,13 @@
         <v>199</v>
       </c>
       <c r="B10" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C10" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,13 +1426,13 @@
         <v>199</v>
       </c>
       <c r="B11" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1445,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1498,7 @@
         <v>199</v>
       </c>
       <c r="G3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1574,12 +1568,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E15" t="s">
         <v>197</v>
@@ -1595,12 +1589,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E18" t="s">
         <v>197</v>
@@ -1616,12 +1610,12 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="E21" t="s">
         <v>197</v>
@@ -1637,12 +1631,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E24" t="s">
         <v>197</v>
@@ -1658,12 +1652,12 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E27" t="s">
         <v>197</v>
@@ -1679,12 +1673,12 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="E30" t="s">
         <v>197</v>
@@ -1700,12 +1694,12 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E33" t="s">
         <v>197</v>
@@ -1721,12 +1715,12 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="E36" t="s">
         <v>197</v>
@@ -1765,7 +1759,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>11</v>
@@ -1812,7 +1806,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1823,7 +1817,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,7 +1828,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,7 +1894,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1911,7 +1905,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1922,7 +1916,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1933,7 +1927,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1944,7 +1938,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2125,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="210" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Small changes to framework
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6110D18-A561-44B0-B36B-00FA82324FBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6853515F-4FE9-42C4-BFE1-D9F38DC70C75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="245">
   <si>
     <t>clause</t>
   </si>
@@ -657,18 +657,12 @@
     <t>'?' + odkSurvey.getHashString('MIF')</t>
   </si>
   <si>
-    <t>MIFVISIT</t>
-  </si>
-  <si>
     <t>Woman in the fertile age - visit</t>
   </si>
   <si>
     <t>Mulher na idade fertil - visita</t>
   </si>
   <si>
-    <t>'?' + odkSurvey.getHashString('MIFVISIT')</t>
-  </si>
-  <si>
     <t>Choose a form</t>
   </si>
   <si>
@@ -705,12 +699,6 @@
     <t>Child Visit</t>
   </si>
   <si>
-    <t>Child visit</t>
-  </si>
-  <si>
-    <t>CHILD</t>
-  </si>
-  <si>
     <t>SCAR</t>
   </si>
   <si>
@@ -781,6 +769,21 @@
   </si>
   <si>
     <t>Grávidas_visitas</t>
+  </si>
+  <si>
+    <t>Crianca</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Crianca_visitas</t>
+  </si>
+  <si>
+    <t>MIF_VISIT</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MIF_VISIT')</t>
   </si>
 </sst>
 </file>
@@ -1186,13 +1189,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>174</v>
@@ -1246,7 +1249,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E7" t="s">
         <v>176</v>
@@ -1257,7 +1260,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1273,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1292,7 @@
         <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1303,10 +1306,10 @@
         <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1317,13 @@
         <v>199</v>
       </c>
       <c r="B3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" t="s">
         <v>202</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>203</v>
-      </c>
-      <c r="D3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,13 +1331,13 @@
         <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,13 +1345,13 @@
         <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,13 +1359,13 @@
         <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,13 +1373,13 @@
         <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,13 +1387,13 @@
         <v>199</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,13 +1401,13 @@
         <v>199</v>
       </c>
       <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" t="s">
         <v>213</v>
-      </c>
-      <c r="C9" t="s">
-        <v>214</v>
-      </c>
-      <c r="D9" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,13 +1415,13 @@
         <v>199</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D10" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,13 +1429,13 @@
         <v>199</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -1445,7 +1448,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1501,7 @@
         <v>199</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1547,12 +1550,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E12" t="s">
         <v>197</v>
@@ -1568,12 +1571,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E15" t="s">
         <v>197</v>
@@ -1589,12 +1592,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E18" t="s">
         <v>197</v>
@@ -1610,12 +1613,12 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E21" t="s">
         <v>197</v>
@@ -1631,12 +1634,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E24" t="s">
         <v>197</v>
@@ -1652,12 +1655,12 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E27" t="s">
         <v>197</v>
@@ -1673,12 +1676,12 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E30" t="s">
         <v>197</v>
@@ -1694,12 +1697,12 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E33" t="s">
         <v>197</v>
@@ -1715,12 +1718,12 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E36" t="s">
         <v>197</v>
@@ -1743,7 +1746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A43F1AA-AE9E-40A3-94B1-695B21603B14}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -1759,7 +1762,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>11</v>
@@ -1806,7 +1809,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1817,7 +1820,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,7 +1831,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,7 +1897,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1905,7 +1908,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1916,7 +1919,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1927,7 +1930,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1938,7 +1941,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,7 +2128,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="210" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed text from initial screens
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6853515F-4FE9-42C4-BFE1-D9F38DC70C75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18302F17-46C2-441F-BB24-604E63EE17BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
   <si>
     <t>clause</t>
   </si>
@@ -272,12 +272,6 @@
     <t>survey_form_identification</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;center&gt;ODK Survey&lt;/center&gt;&lt;hr&gt;&lt;/div&gt;&lt;div&gt;&lt;p&gt;Form name: {{localizeText form_title}}&lt;/p&gt;{{#if form_version}}&lt;p&gt;Form version: {{form_version}}&lt;/p&gt;{{/if}}&lt;hr&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;center&gt;ODK Survey&lt;/center&gt;&lt;hr&gt;&lt;/div&gt;&lt;div&gt;&lt;p&gt;Nome do formulario: {{localizeText form_title}}&lt;/p&gt;{{#if form_version}}&lt;p&gt;Versão do formulário: {{form_version}}&lt;/p&gt;{{/if}}&lt;hr&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>finalize_survey_instance_detail</t>
   </si>
   <si>
@@ -330,37 +324,6 @@
   </si>
   <si>
     <t>opening_survey_instance_detail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     {{#if display_field}}
-        &lt;p&gt;You are at the beginning of the questionaire: &lt;/p&gt;
-        &lt;p&gt;"{{display_field}}"&lt;/p&gt; 
-  {{else}}
-        &lt;p&gt;You are at the start of a new questionaire.&lt;/p&gt;
-  {{/if}}
-        &lt;hr&gt;
-        {{#if last_save_date}}
-            &lt;p&gt;Last saved:&lt;/p&gt; 
-            &lt;p&gt;{{last_save_date}}&lt;/p&gt;
-        {{/if}}
-        &lt;hr&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     
-  {{#if display_field}}
-        &lt;p&gt;Você está no começo do questionário: &lt;/p&gt;
-        &lt;p&gt;"{{display_field}}"&lt;/p&gt; 
-  {{else}}
-        &lt;p&gt;Você está no começo de um novo questionário.&lt;/p&gt;
-  {{/if}}
-        &lt;hr&gt;
-        {{#if last_save_date}}
-            &lt;p&gt;Guardado por última vez:&lt;/p&gt; 
-            &lt;p&gt;{{last_save_date}}&lt;/p&gt;
-        {{/if}}
-        &lt;hr&gt;
-</t>
   </si>
   <si>
     <t>opening_survey_next_button_label</t>
@@ -1189,16 +1152,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1230,37 +1193,37 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1272,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,13 +1249,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1300,142 +1263,142 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
         <v>199</v>
-      </c>
-      <c r="B3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -1464,277 +1427,277 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E18" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G18" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E21" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G21" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G24" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E27" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G30" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E33" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G36" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1746,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A43F1AA-AE9E-40A3-94B1-695B21603B14}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>11</v>
@@ -1809,7 +1772,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1820,7 +1783,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1831,7 +1794,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1897,7 +1860,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1908,7 +1871,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1919,7 +1882,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1930,7 +1893,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1941,7 +1904,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,356 +2017,347 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>